<commit_message>
Fix formula evaluation caching issues (#17854)
 * Use a common FormulaEvaluator
 * Force formula evaluation before conditional rule checks
 * Fixes SHEET-4

Change-Id: I3c1271fbfc35970f7843d8e11be3ae653dc0a121
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1440" windowWidth="24120" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,27 +65,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -463,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -479,10 +459,27 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <f>B3+C3</f>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"AAAAA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix conditional formatting String comparison (#17851)
Fixes SHEET-16

Change-Id: Icb493c2ec116978958d786dd7ce1429a60d94f00
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -65,7 +65,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -446,7 +476,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -473,13 +503,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"AAAAA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"O"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>